<commit_message>
third commit for sending local git to org git
</commit_message>
<xml_diff>
--- a/BULK_API_CONFIG_FILE/Engagement_training_config_file.xlsx
+++ b/BULK_API_CONFIG_FILE/Engagement_training_config_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vamsikkrishna\PycharmProjects\pythonProject1\BULK_API_CONFIG_FILE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99904D9-3582-472B-BFDE-B4A02ACD4D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BDE35F-3F67-4260-B888-7E3751D82D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config_table_flow" sheetId="4" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Pickle_file_locations" sheetId="5" r:id="rId11"/>
     <sheet name="BULK_Pickle_file_locations" sheetId="12" r:id="rId12"/>
     <sheet name="Constraints" sheetId="3" r:id="rId13"/>
+    <sheet name="DB_Status" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SDV_BULK!$A$1:$N$167</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3478" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498" uniqueCount="580">
   <si>
     <t>Sub_process_area</t>
   </si>
@@ -1753,6 +1754,36 @@
   </si>
   <si>
     <t>Data_Display</t>
+  </si>
+  <si>
+    <t>DB_Status_ID</t>
+  </si>
+  <si>
+    <t>DB_Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draft </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draft Generation in Progress </t>
+  </si>
+  <si>
+    <t>Generated Successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while data generation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data posting in progress </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posted Successfully </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while posting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data posting completed with errors </t>
   </si>
 </sst>
 </file>
@@ -2251,10 +2282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35913CC-F43F-446A-A33E-2BA28B349837}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2351,6 +2382,14 @@
         <v>564</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>571</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2362,7 +2401,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2763,6 +2802,126 @@
       </c>
       <c r="E2" t="s">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1DAC0F1-A447-4A4C-B521-3E49B79EFFB8}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>579</v>
       </c>
     </row>
   </sheetData>
@@ -7279,8 +7438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AB707A-3924-4BE5-AFE4-6941D3FA1953}">
   <dimension ref="A1:O333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8470,7 +8629,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>1</v>
       </c>
@@ -8721,7 +8880,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>1</v>
       </c>
@@ -8799,7 +8958,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>1</v>
       </c>
@@ -8838,7 +8997,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
@@ -8918,7 +9077,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>1</v>
       </c>
@@ -8998,7 +9157,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>1</v>
       </c>
@@ -9363,7 +9522,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>1</v>
       </c>
@@ -10212,7 +10371,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>1</v>
       </c>
@@ -10253,7 +10412,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>1</v>
       </c>
@@ -10745,7 +10904,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>1</v>
       </c>
@@ -11114,7 +11273,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>1</v>
       </c>
@@ -11196,7 +11355,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>1</v>
       </c>
@@ -11279,7 +11438,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>1</v>
       </c>
@@ -11611,7 +11770,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>1</v>
       </c>
@@ -11655,7 +11814,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>1</v>
       </c>
@@ -11784,7 +11943,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>1</v>
       </c>
@@ -12158,7 +12317,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>1</v>
       </c>
@@ -12288,7 +12447,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
         <v>1</v>
       </c>
@@ -12314,7 +12473,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
         <v>1</v>
       </c>
@@ -12392,7 +12551,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
         <v>1</v>
       </c>
@@ -12444,7 +12603,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>1</v>
       </c>
@@ -12470,7 +12629,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>1</v>
       </c>
@@ -12496,7 +12655,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>1</v>
       </c>
@@ -12522,7 +12681,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>1</v>
       </c>
@@ -12768,7 +12927,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
         <v>1</v>
       </c>
@@ -12820,7 +12979,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
         <v>1</v>
       </c>
@@ -12968,7 +13127,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
         <v>1</v>
       </c>
@@ -13112,7 +13271,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157" s="4" t="s">
         <v>1</v>
       </c>

</xml_diff>